<commit_message>
Inclusión de imágenes faltantes
Inclusión de imágenes faltantes
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion16/SolicitudGrafica_CN_10_16_CO_REC_10.xlsx
+++ b/fuentes/contenidos/grado10/guion16/SolicitudGrafica_CN_10_16_CO_REC_10.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Dropbox\RECURSOS_CN_10_16_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado10\guion16\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="203">
   <si>
     <t>Fecha:</t>
   </si>
@@ -634,6 +634,9 @@
   </si>
   <si>
     <t>realizar ilustración igual a la imagen guía, q,m, s, y T en itálica</t>
+  </si>
+  <si>
+    <t>Realizar tabla igual a imagen guía, es para ficha de estudiante</t>
   </si>
 </sst>
 </file>
@@ -3052,84 +3055,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>198438</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1657350</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>989013</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="14192250" y="33337501"/>
-          <a:ext cx="1181100" cy="790575"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:schemeClr val="bg2"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>111125</xdr:rowOff>
@@ -3148,7 +3073,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3201,7 +3126,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3250,7 +3175,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3328,7 +3253,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3383,7 +3308,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3436,7 +3361,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3483,7 +3408,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3532,7 +3457,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3610,7 +3535,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3688,7 +3613,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3743,7 +3668,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3798,7 +3723,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3874,7 +3799,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3923,7 +3848,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4001,7 +3926,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4079,7 +4004,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4134,7 +4059,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4187,7 +4112,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4225,7 +4150,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4263,7 +4188,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4276,6 +4201,152 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>39687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1746250</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>1001712</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14319250" y="33178750"/>
+          <a:ext cx="1143000" cy="962025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:schemeClr val="bg2"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1772146</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>1061393</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14049375" y="58999438"/>
+          <a:ext cx="1438771" cy="982018"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -4999,8 +5070,8 @@
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J52" sqref="J52"/>
+      <pane ySplit="9" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -6985,36 +7056,40 @@
         <v>194</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="11" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="B53" s="62"/>
+        <v>IMG44</v>
+      </c>
+      <c r="B53" s="62" t="s">
+        <v>191</v>
+      </c>
       <c r="C53" s="20" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>Recurso F7B</v>
       </c>
       <c r="D53" s="63"/>
       <c r="E53" s="63"/>
-      <c r="F53" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="G53" s="13" t="str">
+      <c r="F53" s="13" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G53" s="13" t="e">
         <f ca="1">IF($F53&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E53,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="H53" s="13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="H53" s="13" t="e">
         <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="I53" s="13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="I53" s="13" t="e">
         <f ca="1">IF(OR($B53&lt;&gt;"",$J53&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E53,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E53,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v/>
+        <v>#N/A</v>
       </c>
       <c r="J53" s="63"/>
-      <c r="K53" s="65"/>
+      <c r="K53" s="65" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="54" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="str">

</xml_diff>